<commit_message>
correção no teste t para uma população - valor_p
</commit_message>
<xml_diff>
--- a/estatistica-basica/actual/banco-items/ht_mean_unknown_var/valor_p/dados.xlsx
+++ b/estatistica-basica/actual/banco-items/ht_mean_unknown_var/valor_p/dados.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A306"/>
+  <dimension ref="A1:A248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -366,1527 +366,1237 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>11.81</v>
+        <v>9.6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>10.55</v>
+        <v>13.61</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>12.45</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>13.34</v>
+        <v>5.63</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>10.61</v>
+        <v>10.32</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>10.75</v>
+        <v>14.17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>14.87</v>
+        <v>14.27</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>15.07</v>
+        <v>9.359999999999999</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>8.48</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>12.48</v>
+        <v>14.69</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>17.06</v>
+        <v>14.69</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>14.08</v>
+        <v>12.31</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>8.789999999999999</v>
+        <v>9.6</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>8.699999999999999</v>
+        <v>11.75</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>14.12</v>
+        <v>7.24</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>11.24</v>
+        <v>9.800000000000001</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>7.85</v>
+        <v>3.58</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>18.21</v>
+        <v>9.800000000000001</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>11.89</v>
+        <v>5.08</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>10.04</v>
+        <v>13.07</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>13.17</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>12.24</v>
+        <v>4.31</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>13.21</v>
+        <v>3.67</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>11.25</v>
+        <v>15.66</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>14.6</v>
+        <v>7.69</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>14.5</v>
+        <v>5.08</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>7.65</v>
+        <v>4.85</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>15.6</v>
+        <v>10.89</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>12.69</v>
+        <v>12.45</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>14.22</v>
+        <v>9.56</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>9.91</v>
+        <v>4.98</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>9.66</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>10.11</v>
+        <v>24.28</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>6.56</v>
+        <v>8.859999999999999</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>11.25</v>
+        <v>6.66</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>15.29</v>
+        <v>13.44</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>14.52</v>
+        <v>15.57</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>16.73</v>
+        <v>9.43</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>13.97</v>
+        <v>7.13</v>
       </c>
     </row>
     <row r="41">
       <c r="A41">
-        <v>10.89</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="42">
       <c r="A42">
-        <v>3.98</v>
+        <v>13.72</v>
       </c>
     </row>
     <row r="43">
       <c r="A43">
-        <v>11.61</v>
+        <v>12.63</v>
       </c>
     </row>
     <row r="44">
       <c r="A44">
-        <v>14.66</v>
+        <v>12.58</v>
       </c>
     </row>
     <row r="45">
       <c r="A45">
-        <v>11.11</v>
+        <v>16.22</v>
       </c>
     </row>
     <row r="46">
       <c r="A46">
-        <v>13.71</v>
+        <v>13.69</v>
       </c>
     </row>
     <row r="47">
       <c r="A47">
-        <v>17.21</v>
+        <v>12.15</v>
       </c>
     </row>
     <row r="48">
       <c r="A48">
-        <v>9.220000000000001</v>
+        <v>11.89</v>
       </c>
     </row>
     <row r="49">
       <c r="A49">
-        <v>8.58</v>
+        <v>5.92</v>
       </c>
     </row>
     <row r="50">
       <c r="A50">
-        <v>12.69</v>
+        <v>15.18</v>
       </c>
     </row>
     <row r="51">
       <c r="A51">
-        <v>8.69</v>
+        <v>11.56</v>
       </c>
     </row>
     <row r="52">
       <c r="A52">
-        <v>12.4</v>
+        <v>6.73</v>
       </c>
     </row>
     <row r="53">
       <c r="A53">
-        <v>12.61</v>
+        <v>10.94</v>
       </c>
     </row>
     <row r="54">
       <c r="A54">
-        <v>12.29</v>
+        <v>7.85</v>
       </c>
     </row>
     <row r="55">
       <c r="A55">
-        <v>11.42</v>
+        <v>14.09</v>
       </c>
     </row>
     <row r="56">
       <c r="A56">
-        <v>15.51</v>
+        <v>9.74</v>
       </c>
     </row>
     <row r="57">
       <c r="A57">
-        <v>19.34</v>
+        <v>12.43</v>
       </c>
     </row>
     <row r="58">
       <c r="A58">
-        <v>4.86</v>
+        <v>15.44</v>
       </c>
     </row>
     <row r="59">
       <c r="A59">
-        <v>17.34</v>
+        <v>14.98</v>
       </c>
     </row>
     <row r="60">
       <c r="A60">
-        <v>15.09</v>
+        <v>5.63</v>
       </c>
     </row>
     <row r="61">
       <c r="A61">
-        <v>19.49</v>
+        <v>18.72</v>
       </c>
     </row>
     <row r="62">
       <c r="A62">
-        <v>10.65</v>
+        <v>11.61</v>
       </c>
     </row>
     <row r="63">
       <c r="A63">
-        <v>13.28</v>
+        <v>14.72</v>
       </c>
     </row>
     <row r="64">
       <c r="A64">
-        <v>15.77</v>
+        <v>10.63</v>
       </c>
     </row>
     <row r="65">
       <c r="A65">
-        <v>12.47</v>
+        <v>16.2</v>
       </c>
     </row>
     <row r="66">
       <c r="A66">
-        <v>14.05</v>
+        <v>11.74</v>
       </c>
     </row>
     <row r="67">
       <c r="A67">
-        <v>13</v>
+        <v>7.41</v>
       </c>
     </row>
     <row r="68">
       <c r="A68">
-        <v>13.87</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="69">
       <c r="A69">
-        <v>13.94</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
       <c r="A70">
-        <v>15.57</v>
+        <v>3.14</v>
       </c>
     </row>
     <row r="71">
       <c r="A71">
-        <v>15.66</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="72">
       <c r="A72">
-        <v>10.98</v>
+        <v>15.71</v>
       </c>
     </row>
     <row r="73">
       <c r="A73">
-        <v>8.9</v>
+        <v>8.529999999999999</v>
       </c>
     </row>
     <row r="74">
       <c r="A74">
-        <v>13.68</v>
+        <v>7.34</v>
       </c>
     </row>
     <row r="75">
       <c r="A75">
-        <v>14.89</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="76">
       <c r="A76">
-        <v>12.32</v>
+        <v>15.29</v>
       </c>
     </row>
     <row r="77">
       <c r="A77">
-        <v>14.4</v>
+        <v>8.949999999999999</v>
       </c>
     </row>
     <row r="78">
       <c r="A78">
-        <v>12.72</v>
+        <v>13.98</v>
       </c>
     </row>
     <row r="79">
       <c r="A79">
-        <v>13.83</v>
+        <v>11.43</v>
       </c>
     </row>
     <row r="80">
       <c r="A80">
-        <v>10.94</v>
+        <v>11.75</v>
       </c>
     </row>
     <row r="81">
       <c r="A81">
-        <v>11.69</v>
+        <v>5.58</v>
       </c>
     </row>
     <row r="82">
       <c r="A82">
-        <v>11.88</v>
+        <v>15.43</v>
       </c>
     </row>
     <row r="83">
       <c r="A83">
-        <v>14.27</v>
+        <v>8.35</v>
       </c>
     </row>
     <row r="84">
       <c r="A84">
-        <v>12.99</v>
+        <v>9.970000000000001</v>
       </c>
     </row>
     <row r="85">
       <c r="A85">
-        <v>5.89</v>
+        <v>10.63</v>
       </c>
     </row>
     <row r="86">
       <c r="A86">
-        <v>12.59</v>
+        <v>16.26</v>
       </c>
     </row>
     <row r="87">
       <c r="A87">
-        <v>14.69</v>
+        <v>21.29</v>
       </c>
     </row>
     <row r="88">
       <c r="A88">
-        <v>15.5</v>
+        <v>10.26</v>
       </c>
     </row>
     <row r="89">
       <c r="A89">
-        <v>12.18</v>
+        <v>14.47</v>
       </c>
     </row>
     <row r="90">
       <c r="A90">
-        <v>7.08</v>
+        <v>6.05</v>
       </c>
     </row>
     <row r="91">
       <c r="A91">
-        <v>7.8</v>
+        <v>7.85</v>
       </c>
     </row>
     <row r="92">
       <c r="A92">
-        <v>8.07</v>
+        <v>12.66</v>
       </c>
     </row>
     <row r="93">
       <c r="A93">
-        <v>18.81</v>
+        <v>13.91</v>
       </c>
     </row>
     <row r="94">
       <c r="A94">
-        <v>4.7</v>
+        <v>19.43</v>
       </c>
     </row>
     <row r="95">
       <c r="A95">
-        <v>14.93</v>
+        <v>-2.68</v>
       </c>
     </row>
     <row r="96">
       <c r="A96">
-        <v>14.48</v>
+        <v>17.52</v>
       </c>
     </row>
     <row r="97">
       <c r="A97">
-        <v>11.06</v>
+        <v>8.470000000000001</v>
       </c>
     </row>
     <row r="98">
       <c r="A98">
-        <v>11.03</v>
+        <v>9.279999999999999</v>
       </c>
     </row>
     <row r="99">
       <c r="A99">
-        <v>12.69</v>
+        <v>7.28</v>
       </c>
     </row>
     <row r="100">
       <c r="A100">
-        <v>10.06</v>
+        <v>7.19</v>
       </c>
     </row>
     <row r="101">
       <c r="A101">
-        <v>9.93</v>
+        <v>2.94</v>
       </c>
     </row>
     <row r="102">
       <c r="A102">
-        <v>12.46</v>
+        <v>7.86</v>
       </c>
     </row>
     <row r="103">
       <c r="A103">
-        <v>15.64</v>
+        <v>12.98</v>
       </c>
     </row>
     <row r="104">
       <c r="A104">
-        <v>13.09</v>
+        <v>6.47</v>
       </c>
     </row>
     <row r="105">
       <c r="A105">
-        <v>10.65</v>
+        <v>4.52</v>
       </c>
     </row>
     <row r="106">
       <c r="A106">
-        <v>11.28</v>
+        <v>7.38</v>
       </c>
     </row>
     <row r="107">
       <c r="A107">
-        <v>9.59</v>
+        <v>9.34</v>
       </c>
     </row>
     <row r="108">
       <c r="A108">
-        <v>8.07</v>
+        <v>12.31</v>
       </c>
     </row>
     <row r="109">
       <c r="A109">
-        <v>13.81</v>
+        <v>7.44</v>
       </c>
     </row>
     <row r="110">
       <c r="A110">
-        <v>10.62</v>
+        <v>7.82</v>
       </c>
     </row>
     <row r="111">
       <c r="A111">
-        <v>15.28</v>
+        <v>16.82</v>
       </c>
     </row>
     <row r="112">
       <c r="A112">
-        <v>10.4</v>
+        <v>8.25</v>
       </c>
     </row>
     <row r="113">
       <c r="A113">
-        <v>16.15</v>
+        <v>13.66</v>
       </c>
     </row>
     <row r="114">
       <c r="A114">
-        <v>8.99</v>
+        <v>14.01</v>
       </c>
     </row>
     <row r="115">
       <c r="A115">
-        <v>9.17</v>
+        <v>1.55</v>
       </c>
     </row>
     <row r="116">
       <c r="A116">
-        <v>12</v>
+        <v>13.2</v>
       </c>
     </row>
     <row r="117">
       <c r="A117">
-        <v>10.96</v>
+        <v>11.36</v>
       </c>
     </row>
     <row r="118">
       <c r="A118">
-        <v>9.65</v>
+        <v>7.59</v>
       </c>
     </row>
     <row r="119">
       <c r="A119">
-        <v>12.38</v>
+        <v>14.44</v>
       </c>
     </row>
     <row r="120">
       <c r="A120">
-        <v>14.1</v>
+        <v>13.34</v>
       </c>
     </row>
     <row r="121">
       <c r="A121">
-        <v>11.25</v>
+        <v>9.94</v>
       </c>
     </row>
     <row r="122">
       <c r="A122">
-        <v>17.08</v>
+        <v>7.27</v>
       </c>
     </row>
     <row r="123">
       <c r="A123">
-        <v>11.44</v>
+        <v>9.98</v>
       </c>
     </row>
     <row r="124">
       <c r="A124">
-        <v>11.12</v>
+        <v>14.58</v>
       </c>
     </row>
     <row r="125">
       <c r="A125">
-        <v>12.7</v>
+        <v>18.05</v>
       </c>
     </row>
     <row r="126">
       <c r="A126">
-        <v>18.71</v>
+        <v>12.12</v>
       </c>
     </row>
     <row r="127">
       <c r="A127">
-        <v>15</v>
+        <v>13.92</v>
       </c>
     </row>
     <row r="128">
       <c r="A128">
-        <v>13.27</v>
+        <v>9.640000000000001</v>
       </c>
     </row>
     <row r="129">
       <c r="A129">
-        <v>8.48</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="130">
       <c r="A130">
-        <v>13.15</v>
+        <v>8.98</v>
       </c>
     </row>
     <row r="131">
       <c r="A131">
-        <v>15.59</v>
+        <v>11.22</v>
       </c>
     </row>
     <row r="132">
       <c r="A132">
-        <v>10.86</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="133">
       <c r="A133">
-        <v>14.04</v>
+        <v>5.14</v>
       </c>
     </row>
     <row r="134">
       <c r="A134">
-        <v>14.37</v>
+        <v>14.97</v>
       </c>
     </row>
     <row r="135">
       <c r="A135">
-        <v>14.63</v>
+        <v>12.82</v>
       </c>
     </row>
     <row r="136">
       <c r="A136">
-        <v>13.2</v>
+        <v>9.470000000000001</v>
       </c>
     </row>
     <row r="137">
       <c r="A137">
-        <v>12.51</v>
+        <v>11.93</v>
       </c>
     </row>
     <row r="138">
       <c r="A138">
-        <v>12.68</v>
+        <v>17.85</v>
       </c>
     </row>
     <row r="139">
       <c r="A139">
-        <v>9.390000000000001</v>
+        <v>17.33</v>
       </c>
     </row>
     <row r="140">
       <c r="A140">
-        <v>7.69</v>
+        <v>16.19</v>
       </c>
     </row>
     <row r="141">
       <c r="A141">
-        <v>13.22</v>
+        <v>2.61</v>
       </c>
     </row>
     <row r="142">
       <c r="A142">
-        <v>13.28</v>
+        <v>10.89</v>
       </c>
     </row>
     <row r="143">
       <c r="A143">
-        <v>15.4</v>
+        <v>15.72</v>
       </c>
     </row>
     <row r="144">
       <c r="A144">
-        <v>13.64</v>
+        <v>11.85</v>
       </c>
     </row>
     <row r="145">
       <c r="A145">
-        <v>11.89</v>
+        <v>16.14</v>
       </c>
     </row>
     <row r="146">
       <c r="A146">
-        <v>13.95</v>
+        <v>12.15</v>
       </c>
     </row>
     <row r="147">
       <c r="A147">
-        <v>15.43</v>
+        <v>-1.05</v>
       </c>
     </row>
     <row r="148">
       <c r="A148">
-        <v>15.37</v>
+        <v>7.69</v>
       </c>
     </row>
     <row r="149">
       <c r="A149">
-        <v>4.86</v>
+        <v>14.21</v>
       </c>
     </row>
     <row r="150">
       <c r="A150">
-        <v>10.61</v>
+        <v>-0.33</v>
       </c>
     </row>
     <row r="151">
       <c r="A151">
-        <v>11.31</v>
+        <v>14.86</v>
       </c>
     </row>
     <row r="152">
       <c r="A152">
-        <v>12.54</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="153">
       <c r="A153">
-        <v>9.380000000000001</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="154">
       <c r="A154">
-        <v>15.2</v>
+        <v>7.06</v>
       </c>
     </row>
     <row r="155">
       <c r="A155">
-        <v>10.78</v>
+        <v>14.48</v>
       </c>
     </row>
     <row r="156">
       <c r="A156">
-        <v>11.98</v>
+        <v>13.79</v>
       </c>
     </row>
     <row r="157">
       <c r="A157">
-        <v>9.57</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="158">
       <c r="A158">
-        <v>13.32</v>
+        <v>13.31</v>
       </c>
     </row>
     <row r="159">
       <c r="A159">
-        <v>12.43</v>
+        <v>10.09</v>
       </c>
     </row>
     <row r="160">
       <c r="A160">
-        <v>9.31</v>
+        <v>10.68</v>
       </c>
     </row>
     <row r="161">
       <c r="A161">
-        <v>10.64</v>
+        <v>7.51</v>
       </c>
     </row>
     <row r="162">
       <c r="A162">
-        <v>17</v>
+        <v>7.63</v>
       </c>
     </row>
     <row r="163">
       <c r="A163">
-        <v>14.07</v>
+        <v>11.88</v>
       </c>
     </row>
     <row r="164">
       <c r="A164">
-        <v>9.18</v>
+        <v>16.58</v>
       </c>
     </row>
     <row r="165">
       <c r="A165">
-        <v>8</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="166">
       <c r="A166">
-        <v>11.7</v>
+        <v>14.03</v>
       </c>
     </row>
     <row r="167">
       <c r="A167">
-        <v>16.48</v>
+        <v>7.88</v>
       </c>
     </row>
     <row r="168">
       <c r="A168">
-        <v>15.95</v>
+        <v>15.41</v>
       </c>
     </row>
     <row r="169">
       <c r="A169">
-        <v>13.95</v>
+        <v>12.05</v>
       </c>
     </row>
     <row r="170">
       <c r="A170">
-        <v>16.57</v>
+        <v>13.74</v>
       </c>
     </row>
     <row r="171">
       <c r="A171">
-        <v>8.84</v>
+        <v>4.29</v>
       </c>
     </row>
     <row r="172">
       <c r="A172">
-        <v>16.54</v>
+        <v>9.460000000000001</v>
       </c>
     </row>
     <row r="173">
       <c r="A173">
-        <v>16.88</v>
+        <v>16.16</v>
       </c>
     </row>
     <row r="174">
       <c r="A174">
-        <v>11.79</v>
+        <v>10.94</v>
       </c>
     </row>
     <row r="175">
       <c r="A175">
-        <v>13.76</v>
+        <v>13.4</v>
       </c>
     </row>
     <row r="176">
       <c r="A176">
-        <v>15.39</v>
+        <v>7.01</v>
       </c>
     </row>
     <row r="177">
       <c r="A177">
-        <v>16.38</v>
+        <v>7.16</v>
       </c>
     </row>
     <row r="178">
       <c r="A178">
-        <v>16.12</v>
+        <v>11.46</v>
       </c>
     </row>
     <row r="179">
       <c r="A179">
-        <v>7.64</v>
+        <v>15.46</v>
       </c>
     </row>
     <row r="180">
       <c r="A180">
-        <v>14.25</v>
+        <v>8.85</v>
       </c>
     </row>
     <row r="181">
       <c r="A181">
-        <v>15.64</v>
+        <v>10.32</v>
       </c>
     </row>
     <row r="182">
       <c r="A182">
-        <v>8.19</v>
+        <v>8.57</v>
       </c>
     </row>
     <row r="183">
       <c r="A183">
-        <v>10.39</v>
+        <v>8.92</v>
       </c>
     </row>
     <row r="184">
       <c r="A184">
-        <v>9.800000000000001</v>
+        <v>10.74</v>
       </c>
     </row>
     <row r="185">
       <c r="A185">
-        <v>13.98</v>
+        <v>12.71</v>
       </c>
     </row>
     <row r="186">
       <c r="A186">
-        <v>9.74</v>
+        <v>-1.89</v>
       </c>
     </row>
     <row r="187">
       <c r="A187">
-        <v>10.72</v>
+        <v>8.449999999999999</v>
       </c>
     </row>
     <row r="188">
       <c r="A188">
-        <v>18.22</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="189">
       <c r="A189">
-        <v>11.55</v>
+        <v>12.92</v>
       </c>
     </row>
     <row r="190">
       <c r="A190">
-        <v>16.75</v>
+        <v>10.69</v>
       </c>
     </row>
     <row r="191">
       <c r="A191">
-        <v>11.16</v>
+        <v>13.1</v>
       </c>
     </row>
     <row r="192">
       <c r="A192">
-        <v>12.56</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="193">
       <c r="A193">
-        <v>13.66</v>
+        <v>17.96</v>
       </c>
     </row>
     <row r="194">
       <c r="A194">
-        <v>14.14</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="195">
       <c r="A195">
-        <v>10.77</v>
+        <v>13.23</v>
       </c>
     </row>
     <row r="196">
       <c r="A196">
-        <v>13.76</v>
+        <v>14.55</v>
       </c>
     </row>
     <row r="197">
       <c r="A197">
-        <v>8.779999999999999</v>
+        <v>7.41</v>
       </c>
     </row>
     <row r="198">
       <c r="A198">
-        <v>7.67</v>
+        <v>7.04</v>
       </c>
     </row>
     <row r="199">
       <c r="A199">
-        <v>10.69</v>
+        <v>8.81</v>
       </c>
     </row>
     <row r="200">
       <c r="A200">
-        <v>11.82</v>
+        <v>13.49</v>
       </c>
     </row>
     <row r="201">
       <c r="A201">
-        <v>15.6</v>
+        <v>14.93</v>
       </c>
     </row>
     <row r="202">
       <c r="A202">
-        <v>20.22</v>
+        <v>9.49</v>
       </c>
     </row>
     <row r="203">
       <c r="A203">
-        <v>9.75</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="204">
       <c r="A204">
-        <v>13.59</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="205">
       <c r="A205">
-        <v>14.63</v>
+        <v>6.62</v>
       </c>
     </row>
     <row r="206">
       <c r="A206">
-        <v>10.46</v>
+        <v>8.609999999999999</v>
       </c>
     </row>
     <row r="207">
       <c r="A207">
-        <v>10.55</v>
+        <v>7.17</v>
       </c>
     </row>
     <row r="208">
       <c r="A208">
-        <v>15.2</v>
+        <v>10.31</v>
       </c>
     </row>
     <row r="209">
       <c r="A209">
-        <v>7.91</v>
+        <v>7.12</v>
       </c>
     </row>
     <row r="210">
       <c r="A210">
-        <v>9.869999999999999</v>
+        <v>6.91</v>
       </c>
     </row>
     <row r="211">
       <c r="A211">
-        <v>12.89</v>
+        <v>9.529999999999999</v>
       </c>
     </row>
     <row r="212">
       <c r="A212">
-        <v>12.43</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="213">
       <c r="A213">
-        <v>15.29</v>
+        <v>6.05</v>
       </c>
     </row>
     <row r="214">
       <c r="A214">
-        <v>10.89</v>
+        <v>10.26</v>
       </c>
     </row>
     <row r="215">
       <c r="A215">
-        <v>13.68</v>
+        <v>18.54</v>
       </c>
     </row>
     <row r="216">
       <c r="A216">
-        <v>11.06</v>
+        <v>17.85</v>
       </c>
     </row>
     <row r="217">
       <c r="A217">
-        <v>11.88</v>
+        <v>9.67</v>
       </c>
     </row>
     <row r="218">
       <c r="A218">
-        <v>8.800000000000001</v>
+        <v>3.51</v>
       </c>
     </row>
     <row r="219">
       <c r="A219">
-        <v>12.52</v>
+        <v>11.03</v>
       </c>
     </row>
     <row r="220">
       <c r="A220">
-        <v>13.03</v>
+        <v>18.17</v>
       </c>
     </row>
     <row r="221">
       <c r="A221">
-        <v>9.970000000000001</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="222">
       <c r="A222">
-        <v>10.26</v>
+        <v>8.720000000000001</v>
       </c>
     </row>
     <row r="223">
       <c r="A223">
-        <v>10.04</v>
+        <v>15.98</v>
       </c>
     </row>
     <row r="224">
       <c r="A224">
-        <v>11.02</v>
+        <v>8.73</v>
       </c>
     </row>
     <row r="225">
       <c r="A225">
-        <v>14.37</v>
+        <v>10.04</v>
       </c>
     </row>
     <row r="226">
       <c r="A226">
-        <v>12.2</v>
+        <v>17.17</v>
       </c>
     </row>
     <row r="227">
       <c r="A227">
-        <v>15.86</v>
+        <v>10.26</v>
       </c>
     </row>
     <row r="228">
       <c r="A228">
-        <v>7.52</v>
+        <v>7.14</v>
       </c>
     </row>
     <row r="229">
       <c r="A229">
-        <v>15.54</v>
+        <v>18.3</v>
       </c>
     </row>
     <row r="230">
       <c r="A230">
-        <v>15.26</v>
+        <v>3.24</v>
       </c>
     </row>
     <row r="231">
       <c r="A231">
-        <v>16.35</v>
+        <v>10.58</v>
       </c>
     </row>
     <row r="232">
       <c r="A232">
-        <v>13.25</v>
+        <v>17.06</v>
       </c>
     </row>
     <row r="233">
       <c r="A233">
-        <v>9.33</v>
+        <v>4.65</v>
       </c>
     </row>
     <row r="234">
       <c r="A234">
-        <v>15.31</v>
+        <v>9.050000000000001</v>
       </c>
     </row>
     <row r="235">
       <c r="A235">
-        <v>12.5</v>
+        <v>14.81</v>
       </c>
     </row>
     <row r="236">
       <c r="A236">
-        <v>8.31</v>
+        <v>4.84</v>
       </c>
     </row>
     <row r="237">
       <c r="A237">
-        <v>14.16</v>
+        <v>6.05</v>
       </c>
     </row>
     <row r="238">
       <c r="A238">
-        <v>14.52</v>
+        <v>10.31</v>
       </c>
     </row>
     <row r="239">
       <c r="A239">
-        <v>9.65</v>
+        <v>11.04</v>
       </c>
     </row>
     <row r="240">
       <c r="A240">
-        <v>12.45</v>
+        <v>13.62</v>
       </c>
     </row>
     <row r="241">
       <c r="A241">
-        <v>10.09</v>
+        <v>9.42</v>
       </c>
     </row>
     <row r="242">
       <c r="A242">
-        <v>15.48</v>
+        <v>5.63</v>
       </c>
     </row>
     <row r="243">
       <c r="A243">
-        <v>10.74</v>
+        <v>12.82</v>
       </c>
     </row>
     <row r="244">
       <c r="A244">
-        <v>9.4</v>
+        <v>10.73</v>
       </c>
     </row>
     <row r="245">
       <c r="A245">
-        <v>6.9</v>
+        <v>13.01</v>
       </c>
     </row>
     <row r="246">
       <c r="A246">
-        <v>12.98</v>
+        <v>12.67</v>
       </c>
     </row>
     <row r="247">
       <c r="A247">
-        <v>11.89</v>
+        <v>3</v>
       </c>
     </row>
     <row r="248">
       <c r="A248">
-        <v>14.02</v>
-      </c>
-    </row>
-    <row r="249">
-      <c r="A249">
-        <v>0.32</v>
-      </c>
-    </row>
-    <row r="250">
-      <c r="A250">
-        <v>9.550000000000001</v>
-      </c>
-    </row>
-    <row r="251">
-      <c r="A251">
-        <v>15.27</v>
-      </c>
-    </row>
-    <row r="252">
-      <c r="A252">
-        <v>14.23</v>
-      </c>
-    </row>
-    <row r="253">
-      <c r="A253">
-        <v>7.48</v>
-      </c>
-    </row>
-    <row r="254">
-      <c r="A254">
-        <v>8.92</v>
-      </c>
-    </row>
-    <row r="255">
-      <c r="A255">
-        <v>9.09</v>
-      </c>
-    </row>
-    <row r="256">
-      <c r="A256">
-        <v>19.57</v>
-      </c>
-    </row>
-    <row r="257">
-      <c r="A257">
-        <v>12.15</v>
-      </c>
-    </row>
-    <row r="258">
-      <c r="A258">
-        <v>6.66</v>
-      </c>
-    </row>
-    <row r="259">
-      <c r="A259">
-        <v>11.38</v>
-      </c>
-    </row>
-    <row r="260">
-      <c r="A260">
-        <v>13.58</v>
-      </c>
-    </row>
-    <row r="261">
-      <c r="A261">
-        <v>13.62</v>
-      </c>
-    </row>
-    <row r="262">
-      <c r="A262">
-        <v>11.24</v>
-      </c>
-    </row>
-    <row r="263">
-      <c r="A263">
-        <v>6.93</v>
-      </c>
-    </row>
-    <row r="264">
-      <c r="A264">
-        <v>15.03</v>
-      </c>
-    </row>
-    <row r="265">
-      <c r="A265">
-        <v>10.95</v>
-      </c>
-    </row>
-    <row r="266">
-      <c r="A266">
-        <v>11.17</v>
-      </c>
-    </row>
-    <row r="267">
-      <c r="A267">
-        <v>16.42</v>
-      </c>
-    </row>
-    <row r="268">
-      <c r="A268">
-        <v>6.45</v>
-      </c>
-    </row>
-    <row r="269">
-      <c r="A269">
-        <v>10.49</v>
-      </c>
-    </row>
-    <row r="270">
-      <c r="A270">
-        <v>10.67</v>
-      </c>
-    </row>
-    <row r="271">
-      <c r="A271">
-        <v>14.59</v>
-      </c>
-    </row>
-    <row r="272">
-      <c r="A272">
-        <v>13.02</v>
-      </c>
-    </row>
-    <row r="273">
-      <c r="A273">
-        <v>11.2</v>
-      </c>
-    </row>
-    <row r="274">
-      <c r="A274">
-        <v>14.99</v>
-      </c>
-    </row>
-    <row r="275">
-      <c r="A275">
-        <v>10.62</v>
-      </c>
-    </row>
-    <row r="276">
-      <c r="A276">
-        <v>14.77</v>
-      </c>
-    </row>
-    <row r="277">
-      <c r="A277">
-        <v>9.359999999999999</v>
-      </c>
-    </row>
-    <row r="278">
-      <c r="A278">
-        <v>13.28</v>
-      </c>
-    </row>
-    <row r="279">
-      <c r="A279">
-        <v>13.08</v>
-      </c>
-    </row>
-    <row r="280">
-      <c r="A280">
-        <v>13.61</v>
-      </c>
-    </row>
-    <row r="281">
-      <c r="A281">
-        <v>15.92</v>
-      </c>
-    </row>
-    <row r="282">
-      <c r="A282">
-        <v>14.72</v>
-      </c>
-    </row>
-    <row r="283">
-      <c r="A283">
-        <v>15.28</v>
-      </c>
-    </row>
-    <row r="284">
-      <c r="A284">
-        <v>12.65</v>
-      </c>
-    </row>
-    <row r="285">
-      <c r="A285">
-        <v>10.91</v>
-      </c>
-    </row>
-    <row r="286">
-      <c r="A286">
-        <v>11.71</v>
-      </c>
-    </row>
-    <row r="287">
-      <c r="A287">
-        <v>8.460000000000001</v>
-      </c>
-    </row>
-    <row r="288">
-      <c r="A288">
-        <v>9.65</v>
-      </c>
-    </row>
-    <row r="289">
-      <c r="A289">
-        <v>13.48</v>
-      </c>
-    </row>
-    <row r="290">
-      <c r="A290">
-        <v>11.98</v>
-      </c>
-    </row>
-    <row r="291">
-      <c r="A291">
-        <v>14.01</v>
-      </c>
-    </row>
-    <row r="292">
-      <c r="A292">
-        <v>7.12</v>
-      </c>
-    </row>
-    <row r="293">
-      <c r="A293">
-        <v>16.86</v>
-      </c>
-    </row>
-    <row r="294">
-      <c r="A294">
-        <v>11.36</v>
-      </c>
-    </row>
-    <row r="295">
-      <c r="A295">
-        <v>11.77</v>
-      </c>
-    </row>
-    <row r="296">
-      <c r="A296">
-        <v>12.87</v>
-      </c>
-    </row>
-    <row r="297">
-      <c r="A297">
-        <v>9.779999999999999</v>
-      </c>
-    </row>
-    <row r="298">
-      <c r="A298">
-        <v>9.35</v>
-      </c>
-    </row>
-    <row r="299">
-      <c r="A299">
-        <v>13.06</v>
-      </c>
-    </row>
-    <row r="300">
-      <c r="A300">
-        <v>15.73</v>
-      </c>
-    </row>
-    <row r="301">
-      <c r="A301">
-        <v>9.75</v>
-      </c>
-    </row>
-    <row r="302">
-      <c r="A302">
-        <v>7.06</v>
-      </c>
-    </row>
-    <row r="303">
-      <c r="A303">
-        <v>11.08</v>
-      </c>
-    </row>
-    <row r="304">
-      <c r="A304">
-        <v>11.4</v>
-      </c>
-    </row>
-    <row r="305">
-      <c r="A305">
-        <v>8.220000000000001</v>
-      </c>
-    </row>
-    <row r="306">
-      <c r="A306">
-        <v>7.7</v>
+        <v>11.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>